<commit_message>
parent schema work in progress : going to discriminator based schema design
</commit_message>
<xml_diff>
--- a/db_model/Schema-csv_Parent_new.xlsx
+++ b/db_model/Schema-csv_Parent_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\abhay\learning\nestjs-onix-bp\babybot\db_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBA0163-C15F-4420-9DD9-3E0AB6EB60B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D245B70-53E8-4A5E-87B0-88FD4D8B4C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{75C39B3C-75EF-4AAC-A875-F75D1A4CEFFA}"/>
   </bookViews>
@@ -565,7 +565,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,10 +765,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -779,13 +779,13 @@
         <v>15</v>
       </c>
       <c r="I10" s="2" t="str">
-        <f t="shared" ref="I10:I13" si="1">_xlfn.CONCAT(A10," : ",B10)</f>
-        <v>created_date : Date</v>
+        <f>_xlfn.CONCAT(A10," : ",B10)</f>
+        <v>created_by : String</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
@@ -799,13 +799,13 @@
         <v>15</v>
       </c>
       <c r="I11" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>created_by : String</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <f>_xlfn.CONCAT(A11," : ",B11)</f>
+        <v>updated_by : String</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>14</v>
@@ -819,16 +819,16 @@
         <v>15</v>
       </c>
       <c r="I12" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>updated_date : Date</v>
+        <f t="shared" ref="I12:I13" si="1">_xlfn.CONCAT(A12," : ",B12)</f>
+        <v>created_date : Date</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -840,10 +840,11 @@
       </c>
       <c r="I13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>updated_by : String</v>
+        <v>updated_date : Date</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>